<commit_message>
Updated BOM With Part Callouts
</commit_message>
<xml_diff>
--- a/Files For Ordering PC Boards/Barebones BOM.xlsx
+++ b/Files For Ordering PC Boards/Barebones BOM.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="20910"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="27795" windowHeight="11820"/>
+    <workbookView xWindow="7360" yWindow="3600" windowWidth="27800" windowHeight="11820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>Schematic Callout</t>
   </si>
@@ -106,13 +111,37 @@
   </si>
   <si>
     <t>10 ohm 1/4 Watt resistor</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>JP6</t>
+  </si>
+  <si>
+    <t>JP1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,20 +485,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.625" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="42.5703125" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.375" customWidth="1"/>
+    <col min="4" max="4" width="42.625" customWidth="1"/>
+    <col min="5" max="5" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -507,6 +536,9 @@
       </c>
     </row>
     <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
       <c r="B3" t="s">
         <v>12</v>
       </c>
@@ -518,6 +550,9 @@
       </c>
     </row>
     <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
@@ -529,6 +564,9 @@
       </c>
     </row>
     <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -540,6 +578,9 @@
       </c>
     </row>
     <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
@@ -551,6 +592,9 @@
       </c>
     </row>
     <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -562,6 +606,9 @@
       </c>
     </row>
     <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>33</v>
+      </c>
       <c r="B8" t="s">
         <v>29</v>
       </c>
@@ -573,6 +620,9 @@
       </c>
     </row>
     <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
       <c r="B9" t="s">
         <v>23</v>
       </c>
@@ -584,6 +634,9 @@
       </c>
     </row>
     <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -616,30 +669,45 @@
     <hyperlink ref="D11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>